<commit_message>
R Record works completed
</commit_message>
<xml_diff>
--- a/R Programming/Practical Program List.xlsx
+++ b/R Programming/Practical Program List.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MCA\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning-Programming-\R Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="67">
   <si>
     <t>S.No</t>
   </si>
@@ -367,6 +367,24 @@
 Survival Analysis Using Python
 i) vector Data
 ii) Data From CSV</t>
+  </si>
+  <si>
+    <t>Rigen</t>
+  </si>
+  <si>
+    <t>Saran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index Page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeya </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mithilan </t>
+  </si>
+  <si>
+    <t>Piere</t>
   </si>
 </sst>
 </file>
@@ -519,6 +537,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -534,26 +561,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -837,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,19 +865,19 @@
     <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="147.7109375" style="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="10.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -877,12 +895,12 @@
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
       <c r="B3" s="5">
@@ -902,7 +920,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -915,10 +933,10 @@
       <c r="E4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="17"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="5">
         <v>3</v>
       </c>
@@ -931,10 +949,10 @@
       <c r="E5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -947,10 +965,10 @@
       <c r="E6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -963,10 +981,10 @@
       <c r="E7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="18"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="5">
         <v>6</v>
       </c>
@@ -984,7 +1002,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="5">
         <v>7</v>
       </c>
@@ -997,10 +1015,10 @@
       <c r="E9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="5">
         <v>8</v>
       </c>
@@ -1018,7 +1036,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="11">
         <v>2</v>
       </c>
       <c r="B11" s="5">
@@ -1033,10 +1051,10 @@
       <c r="E11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="5">
         <v>10</v>
       </c>
@@ -1054,7 +1072,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="5">
         <v>11</v>
       </c>
@@ -1067,10 +1085,10 @@
       <c r="E13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="18"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="5">
         <v>12</v>
       </c>
@@ -1088,7 +1106,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5">
         <v>13</v>
       </c>
@@ -1101,10 +1119,10 @@
       <c r="E15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="18"/>
+      <c r="F15" s="17"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="11">
         <v>3</v>
       </c>
       <c r="B16" s="5">
@@ -1124,7 +1142,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="5">
         <v>15</v>
       </c>
@@ -1137,10 +1155,10 @@
       <c r="E17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="17"/>
+      <c r="F17" s="18"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="5">
         <v>16</v>
       </c>
@@ -1153,10 +1171,10 @@
       <c r="E18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="17"/>
+      <c r="F18" s="18"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="5">
         <v>17</v>
       </c>
@@ -1169,10 +1187,10 @@
       <c r="E19" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="17"/>
+      <c r="F19" s="18"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="5">
         <v>18</v>
       </c>
@@ -1185,10 +1203,10 @@
       <c r="E20" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="18"/>
+      <c r="F20" s="17"/>
     </row>
     <row r="21" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="5">
         <v>19</v>
       </c>
@@ -1201,12 +1219,12 @@
       <c r="E21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="9" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="5">
         <v>20</v>
       </c>
@@ -1224,7 +1242,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="5">
         <v>21</v>
       </c>
@@ -1237,10 +1255,10 @@
       <c r="E23" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F23" s="17"/>
+      <c r="F23" s="18"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="5">
         <v>22</v>
       </c>
@@ -1253,10 +1271,10 @@
       <c r="E24" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F24" s="18"/>
+      <c r="F24" s="17"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="5">
         <v>23</v>
       </c>
@@ -1274,71 +1292,91 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="5">
         <v>24</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="17"/>
+      <c r="D26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="18"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="5">
         <v>25</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="18"/>
+      <c r="D27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="17"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
+      <c r="A28" s="12"/>
       <c r="B28" s="5">
         <v>26</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="14" t="s">
+      <c r="D28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
+      <c r="A29" s="12"/>
       <c r="B29" s="5">
         <v>27</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="F29" s="16" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="5">
         <v>28</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="18"/>
+      <c r="D30" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="17"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
+      <c r="A31" s="11">
         <v>4</v>
       </c>
       <c r="B31" s="5">
@@ -1353,48 +1391,66 @@
       <c r="E31" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="9" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="5">
         <v>30</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="14"/>
+      <c r="D32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="5">
         <v>31</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="14"/>
+      <c r="D33" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="5">
         <v>32</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="14"/>
+      <c r="D34" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="8">
+      <c r="A35" s="11">
         <v>5</v>
       </c>
       <c r="B35" s="5">
@@ -1403,177 +1459,244 @@
       <c r="C35" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="14"/>
+      <c r="D35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="5">
         <v>34</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="14"/>
+      <c r="D36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
+      <c r="A37" s="12"/>
       <c r="B37" s="5">
         <v>35</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="14"/>
+      <c r="D37" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
+      <c r="A38" s="12"/>
       <c r="B38" s="5">
         <v>36</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="14"/>
+      <c r="D38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
+      <c r="A39" s="12"/>
       <c r="B39" s="5">
         <v>37</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="14"/>
+      <c r="D39" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
+      <c r="A40" s="12"/>
       <c r="B40" s="5">
         <v>38</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="14"/>
+      <c r="D40" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
+      <c r="A41" s="12"/>
       <c r="B41" s="3">
         <v>39</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="14"/>
+      <c r="D41" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="42" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
+      <c r="A42" s="12"/>
       <c r="B42" s="3">
         <v>40</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="14"/>
+      <c r="D42" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="43" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
+      <c r="A43" s="12"/>
       <c r="B43" s="3">
         <v>41</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="14"/>
+      <c r="D43" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
+      <c r="A44" s="12"/>
       <c r="B44" s="3">
         <v>42</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="14" t="s">
+      <c r="D44" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F44" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="9"/>
+      <c r="A45" s="12"/>
       <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="14"/>
+      <c r="C45" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
+      <c r="A46" s="12"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="14"/>
+      <c r="F46" s="9"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="9"/>
+      <c r="A47" s="12"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
-      <c r="F47" s="14"/>
+      <c r="F47" s="9"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
+      <c r="A48" s="12"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="14"/>
+      <c r="F48" s="9"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="9"/>
+      <c r="A49" s="12"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="14"/>
+      <c r="F49" s="9"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
+      <c r="A50" s="12"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="14"/>
+      <c r="F50" s="9"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="10"/>
+      <c r="A51" s="13"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
-      <c r="F51" s="14"/>
+      <c r="F51" s="9"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:F51"/>
   <mergeCells count="15">
     <mergeCell ref="A35:A51"/>
     <mergeCell ref="A1:F1"/>

</xml_diff>